<commit_message>
updated names of ingredients
</commit_message>
<xml_diff>
--- a/bulk-upload-templates/en/EN_E-Label_Template.xlsx
+++ b/bulk-upload-templates/en/EN_E-Label_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gigi/Desktop/Imero/e-label.io/bulk-upload-templates/en/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbauer/workspace/vs_code/misc/e-label.io/bulk-upload-templates/en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8F1E49-EA2F-024D-BA16-CA20946BFD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F284D372-11AF-6546-98EE-7E5DB7ADFBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="15920" xr2:uid="{42B7CF4C-2976-4744-81A6-4766AD4B0A9A}"/>
   </bookViews>
@@ -126,12 +126,6 @@
     <t>Packaged under protective atmosphere</t>
   </si>
   <si>
-    <t>Tartaric acid (L(+)-)</t>
-  </si>
-  <si>
-    <t>Malic acid (D,L-; L-)</t>
-  </si>
-  <si>
     <t>Lactic acid</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>Example wine</t>
+  </si>
+  <si>
+    <t>Tartaric acid</t>
+  </si>
+  <si>
+    <t>Malic acid</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,9 +462,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -502,7 +502,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -608,7 +608,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,7 +750,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -837,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="31">
         <v>2023</v>
@@ -846,7 +846,7 @@
         <v>750</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" s="32">
         <v>12.3</v>
@@ -861,7 +861,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
@@ -18836,7 +18836,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18913,48 +18913,48 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" s="36"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K18" s="36"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -18964,38 +18964,38 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="36"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K23" s="36"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>